<commit_message>
design the structure of the website and create the relation folders and files and so on
</commit_message>
<xml_diff>
--- a/document/数据库设计/危废仓储管理系统数据库设计.xlsx
+++ b/document/数据库设计/危废仓储管理系统数据库设计.xlsx
@@ -102,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>主键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RFID标签编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -155,6 +151,10 @@
   </si>
   <si>
     <t>外键fk_waste_id_receiving，waste表的主键waste_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键，自动递增</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -610,22 +610,22 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +639,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -693,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -701,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -737,7 +737,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -764,10 +764,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -791,7 +791,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -842,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -886,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -894,10 +894,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -913,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
modify the database and add the android function map
</commit_message>
<xml_diff>
--- a/document/数据库设计/危废仓储管理系统数据库设计.xlsx
+++ b/document/数据库设计/危废仓储管理系统数据库设计.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="仓储管理系统数据库说明" sheetId="4" r:id="rId1"/>
     <sheet name="生产单位仓储表" sheetId="1" r:id="rId2"/>
     <sheet name="接受单位仓储表" sheetId="6" r:id="rId3"/>
+    <sheet name="危废品状态" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>当生产单位注册审核通过后，自动生成一张仓储表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,6 +156,110 @@
   </si>
   <si>
     <t>主键，自动递增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_date_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>del_date_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RFID标签编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0：在库，1：出库，2，接受</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当危废品与RFID标签绑定，写入危废品状态表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表名：rfid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要作用，描述RFID标签的状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>此标签记录的总数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键fk_waste_id_rfid，waste表的主键waste_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -186,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -209,13 +314,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -224,74 +343,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -308,7 +359,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -587,15 +638,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B8"/>
+  <dimension ref="B2:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="46.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.15">
@@ -626,6 +677,21 @@
     <row r="8" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -636,10 +702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -757,7 +823,9 @@
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
@@ -779,6 +847,37 @@
         <v>20</v>
       </c>
       <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -788,10 +887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -929,6 +1028,219 @@
       </c>
       <c r="G6" s="1"/>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="7" max="7" width="53.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>255</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>